<commit_message>
Create framework for ALFOC model
</commit_message>
<xml_diff>
--- a/Overview - Video Games.xlsx
+++ b/Overview - Video Games.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376F6DCA-71C4-45CA-B06B-27EAA76765CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82E7593-5895-4ACB-A192-003EEF3DA981}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{241F2393-9455-43D4-B289-8A800D465992}"/>
   </bookViews>
@@ -19,6 +19,7 @@
   <externalReferences>
     <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="614">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="618">
   <si>
     <r>
       <t>▴</t>
@@ -1913,17 +1914,28 @@
   <si>
     <t>IPO</t>
   </si>
+  <si>
+    <t>Focus Entertainment SA</t>
+  </si>
+  <si>
+    <t>S/O</t>
+  </si>
+  <si>
+    <t>Normalised to Pound Sterling (GBP)</t>
+  </si>
+  <si>
+    <t>2023 E</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="164" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
-    <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2030,8 +2042,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="4"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2083,6 +2102,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2219,7 +2244,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2377,9 +2402,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2406,6 +2428,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2537,6 +2568,55 @@
         </row>
       </sheetData>
       <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="6">
+          <cell r="C6">
+            <v>33.75</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="C7">
+            <v>6.16</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="C8">
+            <v>207.9</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="C11">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="C12">
+            <v>207.9</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="C23" t="str">
+            <v>Paris, France</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="C24">
+            <v>1996</v>
+          </cell>
+        </row>
+      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -7655,13 +7735,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EA11F49-38A5-4A76-81B0-A144DE239010}">
-  <dimension ref="A2:AF21"/>
+  <dimension ref="A1:AH21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomRight" activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7672,19 +7752,28 @@
     <col min="4" max="4" width="10.85546875" style="43" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="43"/>
     <col min="6" max="6" width="11.7109375" style="54" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="9.140625" style="54"/>
-    <col min="10" max="11" width="9.140625" style="43"/>
-    <col min="12" max="13" width="9.140625" style="62"/>
-    <col min="14" max="24" width="9.140625" style="43"/>
-    <col min="25" max="28" width="9.140625" style="54"/>
-    <col min="29" max="29" width="9.140625" style="43"/>
-    <col min="30" max="30" width="9.140625" style="51"/>
+    <col min="7" max="10" width="9.140625" style="66"/>
+    <col min="11" max="12" width="9.140625" style="43"/>
+    <col min="13" max="14" width="9.140625" style="61"/>
+    <col min="15" max="25" width="9.140625" style="43"/>
+    <col min="26" max="30" width="9.140625" style="54"/>
     <col min="31" max="31" width="9.140625" style="43"/>
-    <col min="32" max="32" width="14.7109375" style="43" bestFit="1" customWidth="1"/>
-    <col min="33" max="16384" width="9.140625" style="43"/>
+    <col min="32" max="32" width="9.140625" style="51"/>
+    <col min="33" max="33" width="9.140625" style="43"/>
+    <col min="34" max="34" width="14.7109375" style="43" bestFit="1" customWidth="1"/>
+    <col min="35" max="16384" width="9.140625" style="43"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:32" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="F1" s="67" t="s">
+        <v>616</v>
+      </c>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+    </row>
+    <row r="2" spans="1:34" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="43"/>
       <c r="B2" s="44" t="s">
         <v>567</v>
@@ -7701,92 +7790,98 @@
       <c r="F2" s="53" t="s">
         <v>570</v>
       </c>
-      <c r="G2" s="53" t="s">
+      <c r="G2" s="65" t="s">
+        <v>615</v>
+      </c>
+      <c r="H2" s="65" t="s">
         <v>571</v>
       </c>
-      <c r="H2" s="53" t="s">
+      <c r="I2" s="65" t="s">
         <v>572</v>
       </c>
-      <c r="I2" s="53" t="s">
+      <c r="J2" s="65" t="s">
         <v>573</v>
       </c>
-      <c r="J2" s="45" t="s">
+      <c r="K2" s="45" t="s">
         <v>574</v>
       </c>
-      <c r="K2" s="45" t="s">
+      <c r="L2" s="45" t="s">
         <v>610</v>
       </c>
-      <c r="L2" s="61" t="s">
+      <c r="M2" s="60" t="s">
         <v>611</v>
       </c>
-      <c r="M2" s="61" t="s">
+      <c r="N2" s="60" t="s">
         <v>612</v>
       </c>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45" t="s">
+      <c r="O2" s="45"/>
+      <c r="P2" s="45" t="s">
         <v>597</v>
       </c>
-      <c r="P2" s="45" t="s">
+      <c r="Q2" s="45" t="s">
         <v>598</v>
       </c>
-      <c r="Q2" s="45" t="s">
+      <c r="R2" s="45" t="s">
         <v>599</v>
       </c>
-      <c r="S2" s="45" t="s">
+      <c r="T2" s="45" t="s">
         <v>604</v>
       </c>
-      <c r="T2" s="45" t="s">
+      <c r="U2" s="45" t="s">
         <v>605</v>
       </c>
-      <c r="U2" s="45" t="s">
+      <c r="V2" s="45" t="s">
         <v>609</v>
       </c>
-      <c r="V2" s="45" t="s">
+      <c r="W2" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="W2" s="45" t="s">
+      <c r="X2" s="45" t="s">
         <v>608</v>
       </c>
-      <c r="Y2" s="53" t="s">
+      <c r="Z2" s="53" t="s">
+        <v>617</v>
+      </c>
+      <c r="AA2" s="53" t="s">
         <v>600</v>
       </c>
-      <c r="Z2" s="53" t="s">
+      <c r="AB2" s="53" t="s">
         <v>601</v>
       </c>
-      <c r="AA2" s="53" t="s">
+      <c r="AC2" s="53" t="s">
         <v>602</v>
       </c>
-      <c r="AB2" s="53" t="s">
+      <c r="AD2" s="53" t="s">
         <v>603</v>
       </c>
-      <c r="AD2" s="45" t="s">
+      <c r="AF2" s="45" t="s">
         <v>613</v>
       </c>
-      <c r="AE2" s="44" t="s">
+      <c r="AG2" s="44" t="s">
         <v>607</v>
       </c>
-      <c r="AF2" s="45" t="s">
+      <c r="AH2" s="45" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
       <c r="C3" s="46"/>
       <c r="D3" s="51"/>
       <c r="E3" s="51"/>
-      <c r="O3" s="51"/>
       <c r="P3" s="51"/>
       <c r="Q3" s="51"/>
-      <c r="AE3" s="51"/>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="R3" s="51"/>
+      <c r="AG3" s="51"/>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
       <c r="D4" s="51"/>
       <c r="E4" s="51"/>
-      <c r="O4" s="51"/>
       <c r="P4" s="51"/>
       <c r="Q4" s="51"/>
-      <c r="AE4" s="51"/>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="R4" s="51"/>
+      <c r="AG4" s="51"/>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B5" s="43" t="s">
         <v>586</v>
       </c>
@@ -7799,12 +7894,12 @@
       <c r="E5" s="51" t="s">
         <v>588</v>
       </c>
-      <c r="O5" s="51"/>
       <c r="P5" s="51"/>
       <c r="Q5" s="51"/>
-      <c r="AE5" s="51"/>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="R5" s="51"/>
+      <c r="AG5" s="51"/>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B6" s="43" t="s">
         <v>577</v>
       </c>
@@ -7817,12 +7912,12 @@
       <c r="E6" s="51" t="s">
         <v>588</v>
       </c>
-      <c r="O6" s="51"/>
       <c r="P6" s="51"/>
       <c r="Q6" s="51"/>
-      <c r="AE6" s="51"/>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="R6" s="51"/>
+      <c r="AG6" s="51"/>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B7" s="43" t="s">
         <v>578</v>
       </c>
@@ -7835,12 +7930,12 @@
       <c r="E7" s="51" t="s">
         <v>588</v>
       </c>
-      <c r="O7" s="51"/>
       <c r="P7" s="51"/>
       <c r="Q7" s="51"/>
-      <c r="AE7" s="51"/>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="R7" s="51"/>
+      <c r="AG7" s="51"/>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B8" s="43" t="s">
         <v>81</v>
       </c>
@@ -7853,12 +7948,12 @@
       <c r="E8" s="51" t="s">
         <v>589</v>
       </c>
-      <c r="O8" s="51"/>
       <c r="P8" s="51"/>
       <c r="Q8" s="51"/>
-      <c r="AE8" s="51"/>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="R8" s="51"/>
+      <c r="AG8" s="51"/>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B9" s="43" t="s">
         <v>580</v>
       </c>
@@ -7871,12 +7966,12 @@
       <c r="E9" s="51" t="s">
         <v>579</v>
       </c>
-      <c r="O9" s="51"/>
       <c r="P9" s="51"/>
       <c r="Q9" s="51"/>
-      <c r="AE9" s="51"/>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="R9" s="51"/>
+      <c r="AG9" s="51"/>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B10" s="43" t="s">
         <v>127</v>
       </c>
@@ -7885,16 +7980,16 @@
       </c>
       <c r="D10" s="51"/>
       <c r="E10" s="51"/>
-      <c r="J10" s="51"/>
       <c r="K10" s="51"/>
-      <c r="L10" s="63"/>
-      <c r="M10" s="63"/>
-      <c r="N10" s="51"/>
+      <c r="L10" s="51"/>
+      <c r="M10" s="62"/>
+      <c r="N10" s="62"/>
       <c r="O10" s="51"/>
       <c r="P10" s="51"/>
-      <c r="AE10" s="51"/>
-    </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="Q10" s="51"/>
+      <c r="AG10" s="51"/>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B11" s="43" t="s">
         <v>186</v>
       </c>
@@ -7903,16 +7998,16 @@
       </c>
       <c r="D11" s="51"/>
       <c r="E11" s="51"/>
-      <c r="J11" s="51"/>
       <c r="K11" s="51"/>
-      <c r="L11" s="63"/>
-      <c r="M11" s="63"/>
-      <c r="N11" s="51"/>
+      <c r="L11" s="51"/>
+      <c r="M11" s="62"/>
+      <c r="N11" s="62"/>
       <c r="O11" s="51"/>
       <c r="P11" s="51"/>
-      <c r="AE11" s="51"/>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="Q11" s="51"/>
+      <c r="AG11" s="51"/>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B12" s="52" t="s">
         <v>196</v>
       </c>
@@ -7925,49 +8020,49 @@
       <c r="E12" s="51" t="s">
         <v>596</v>
       </c>
-      <c r="F12" s="56">
+      <c r="F12" s="55">
         <f>[1]Main!$C$6</f>
         <v>4.9249999999999998</v>
       </c>
-      <c r="G12" s="55">
+      <c r="H12" s="66">
         <f>[1]Main!$C$8</f>
         <v>194.14349999999999</v>
       </c>
-      <c r="H12" s="55">
+      <c r="I12" s="66">
         <f>[1]Main!$C$11</f>
         <v>0</v>
       </c>
-      <c r="I12" s="55">
+      <c r="J12" s="66">
         <f>[1]Main!$C$12</f>
         <v>194.14349999999999</v>
       </c>
-      <c r="J12" s="51"/>
       <c r="K12" s="51"/>
-      <c r="L12" s="63"/>
-      <c r="M12" s="63"/>
-      <c r="N12" s="51"/>
-      <c r="O12" s="51">
+      <c r="L12" s="51"/>
+      <c r="M12" s="62"/>
+      <c r="N12" s="62"/>
+      <c r="O12" s="51"/>
+      <c r="P12" s="51">
         <f>[1]Main!$C$25</f>
         <v>0</v>
       </c>
-      <c r="P12" s="51">
+      <c r="Q12" s="51">
         <f>[1]Main!$C$26</f>
         <v>0</v>
       </c>
-      <c r="Q12" s="51">
+      <c r="R12" s="51">
         <f>[1]Main!$C$27</f>
         <v>0</v>
       </c>
-      <c r="AE12" s="51">
+      <c r="AG12" s="51">
         <f>[1]Main!$C$24</f>
         <v>1994</v>
       </c>
-      <c r="AF12" s="51" t="str">
+      <c r="AH12" s="51" t="str">
         <f>[1]Main!$C$23</f>
         <v>Cambridge, UK</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A13" s="43" t="s">
         <v>575</v>
       </c>
@@ -7981,31 +8076,75 @@
         <v>595</v>
       </c>
       <c r="E13" s="51"/>
-      <c r="J13" s="51"/>
       <c r="K13" s="51"/>
-      <c r="L13" s="63"/>
-      <c r="M13" s="63"/>
-      <c r="N13" s="51"/>
+      <c r="L13" s="51"/>
+      <c r="M13" s="62"/>
+      <c r="N13" s="62"/>
       <c r="O13" s="51"/>
       <c r="P13" s="51"/>
-      <c r="AE13" s="51"/>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="B14" s="43" t="s">
+      <c r="Q13" s="51"/>
+      <c r="AG13" s="51"/>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="B14" s="52" t="s">
         <v>581</v>
       </c>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="J14" s="51"/>
+      <c r="C14" s="43" t="s">
+        <v>614</v>
+      </c>
+      <c r="D14" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" s="51" t="s">
+        <v>579</v>
+      </c>
+      <c r="F14" s="54">
+        <f>[3]Main!$C$6*E21</f>
+        <v>28.349999999999998</v>
+      </c>
+      <c r="G14" s="66">
+        <f>[3]Main!$C$7</f>
+        <v>6.16</v>
+      </c>
+      <c r="H14" s="66">
+        <f>[3]Main!$C$8*$E$21</f>
+        <v>174.636</v>
+      </c>
+      <c r="I14" s="66">
+        <f>[3]Main!$C$11*$E$21</f>
+        <v>0</v>
+      </c>
+      <c r="J14" s="66">
+        <f>[3]Main!$C$12*$E$21</f>
+        <v>174.636</v>
+      </c>
       <c r="K14" s="51"/>
-      <c r="L14" s="63"/>
-      <c r="M14" s="63"/>
-      <c r="N14" s="51"/>
+      <c r="L14" s="51"/>
+      <c r="M14" s="62"/>
+      <c r="N14" s="62"/>
       <c r="O14" s="51"/>
-      <c r="P14" s="51"/>
-      <c r="AE14" s="51"/>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="P14" s="51">
+        <f>[3]Main!$C$27</f>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="51">
+        <f>[3]Main!$C$28</f>
+        <v>0</v>
+      </c>
+      <c r="R14" s="51">
+        <f>[3]Main!$C$29</f>
+        <v>0</v>
+      </c>
+      <c r="AG14" s="51">
+        <f>[3]Main!$C$24</f>
+        <v>1996</v>
+      </c>
+      <c r="AH14" s="51" t="str">
+        <f>[3]Main!$C$23</f>
+        <v>Paris, France</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B15" s="52" t="s">
         <v>593</v>
       </c>
@@ -8018,53 +8157,53 @@
       <c r="E15" s="51" t="s">
         <v>596</v>
       </c>
-      <c r="F15" s="57">
+      <c r="F15" s="56">
         <f>[2]Main!$C$6</f>
         <v>1.155</v>
       </c>
-      <c r="G15" s="55">
+      <c r="H15" s="66">
         <f>[2]Main!$C$8</f>
         <v>235.07715000000002</v>
       </c>
-      <c r="H15" s="55">
+      <c r="I15" s="66">
         <f>[2]Main!$C$11</f>
         <v>0</v>
       </c>
-      <c r="I15" s="55">
+      <c r="J15" s="66">
         <f>[2]Main!$C$12</f>
         <v>235.07715000000002</v>
       </c>
-      <c r="O15" s="51">
+      <c r="P15" s="51">
         <f>[2]Main!$C$25</f>
         <v>10</v>
       </c>
-      <c r="P15" s="51">
+      <c r="Q15" s="51">
         <f>[2]Main!$C$26</f>
         <v>70</v>
       </c>
-      <c r="Q15" s="51">
+      <c r="R15" s="51">
         <f>[2]Main!$C$27</f>
         <v>30</v>
       </c>
-      <c r="AE15" s="51">
+      <c r="AG15" s="51">
         <f>[2]Main!$C$24</f>
         <v>2011</v>
       </c>
-      <c r="AF15" s="51" t="str">
+      <c r="AH15" s="51" t="str">
         <f>[2]Main!$C$23</f>
         <v>Washington, US</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
       <c r="D16" s="51"/>
       <c r="E16" s="51"/>
     </row>
     <row r="19" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D19" s="64" t="s">
+      <c r="D19" s="63" t="s">
         <v>582</v>
       </c>
-      <c r="E19" s="65"/>
-      <c r="F19" s="58" t="s">
+      <c r="E19" s="64"/>
+      <c r="F19" s="57" t="s">
         <v>583</v>
       </c>
     </row>
@@ -8075,7 +8214,7 @@
       <c r="E20" s="48">
         <v>0.8458</v>
       </c>
-      <c r="F20" s="59">
+      <c r="F20" s="58">
         <f>1/E20</f>
         <v>1.1823126034523528</v>
       </c>
@@ -8087,19 +8226,22 @@
       <c r="E21" s="50">
         <v>0.84</v>
       </c>
-      <c r="F21" s="60">
+      <c r="F21" s="59">
         <f>1/E21</f>
         <v>1.1904761904761905</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F1:J1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B15" r:id="rId1" xr:uid="{492A76F4-4882-4A78-B48A-FE2771E6353E}"/>
     <hyperlink ref="B12" r:id="rId2" xr:uid="{FF627AC4-0649-433C-9977-CAE6BE5385C4}"/>
+    <hyperlink ref="B14" r:id="rId3" xr:uid="{7B76C08B-C15A-49CB-8685-38243193D2C8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="125" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Create & start £TM17
</commit_message>
<xml_diff>
--- a/Overview - Video Games.xlsx
+++ b/Overview - Video Games.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855BCE8E-98FC-4FCA-ABF8-A9D824794792}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B57EB75-1B40-4DC1-B5E1-A8FBA42F8709}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{241F2393-9455-43D4-B289-8A800D465992}"/>
   </bookViews>
@@ -21,6 +21,7 @@
     <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="618">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="619">
   <si>
     <r>
       <t>▴</t>
@@ -1927,14 +1928,18 @@
   <si>
     <t>2023 E</t>
   </si>
+  <si>
+    <t>Employees</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="164" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
+    <numFmt numFmtId="166" formatCode="0.0\x"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -2245,7 +2250,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2440,6 +2445,12 @@
     <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2463,18 +2474,22 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
-      <sheetName val="Financial Model"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="6">
           <cell r="C6">
-            <v>4.9249999999999998</v>
+            <v>141.83000000000001</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="C7">
+            <v>169.83</v>
           </cell>
         </row>
         <row r="8">
           <cell r="C8">
-            <v>194.14349999999999</v>
+            <v>24086.988900000004</v>
           </cell>
         </row>
         <row r="11">
@@ -2484,30 +2499,20 @@
         </row>
         <row r="12">
           <cell r="C12">
-            <v>194.14349999999999</v>
+            <v>24086.988900000004</v>
           </cell>
         </row>
         <row r="23">
           <cell r="C23" t="str">
-            <v>Cambridge, UK</v>
+            <v>NYC, NY</v>
           </cell>
         </row>
         <row r="24">
           <cell r="C24">
-            <v>1994</v>
+            <v>1993</v>
           </cell>
         </row>
-        <row r="25">
-          <cell r="C25"/>
-        </row>
-        <row r="26">
-          <cell r="C26"/>
-        </row>
-        <row r="27">
-          <cell r="C27"/>
-        </row>
       </sheetData>
-      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2518,22 +2523,23 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
+      <sheetName val="Financial Model"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="6">
           <cell r="C6">
-            <v>33.75</v>
+            <v>2.75</v>
           </cell>
         </row>
         <row r="7">
           <cell r="C7">
-            <v>6.16</v>
+            <v>145.80000000000001</v>
           </cell>
         </row>
         <row r="8">
           <cell r="C8">
-            <v>207.9</v>
+            <v>400.95000000000005</v>
           </cell>
         </row>
         <row r="11">
@@ -2543,20 +2549,44 @@
         </row>
         <row r="12">
           <cell r="C12">
-            <v>207.9</v>
+            <v>400.95000000000005</v>
           </cell>
         </row>
         <row r="23">
           <cell r="C23" t="str">
-            <v>Paris, France</v>
+            <v>Wakefield, UK</v>
           </cell>
         </row>
         <row r="24">
           <cell r="C24">
-            <v>1996</v>
+            <v>1990</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="C25">
+            <v>2018</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="C31">
+            <v>438</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="C33" t="str">
+            <v>H123</v>
+          </cell>
+          <cell r="D33">
+            <v>45188</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="C38">
+            <v>1.5479168086347954</v>
           </cell>
         </row>
       </sheetData>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2628,22 +2658,18 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
+      <sheetName val="Financial Model"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="6">
           <cell r="C6">
-            <v>141.83000000000001</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="C7">
-            <v>169.83</v>
+            <v>4.9249999999999998</v>
           </cell>
         </row>
         <row r="8">
           <cell r="C8">
-            <v>24086.988900000004</v>
+            <v>194.14349999999999</v>
           </cell>
         </row>
         <row r="11">
@@ -2653,18 +2679,86 @@
         </row>
         <row r="12">
           <cell r="C12">
-            <v>24086.988900000004</v>
+            <v>194.14349999999999</v>
           </cell>
         </row>
         <row r="23">
           <cell r="C23" t="str">
-            <v>NYC, NY</v>
+            <v>Cambridge, UK</v>
           </cell>
         </row>
         <row r="24">
           <cell r="C24">
-            <v>1993</v>
+            <v>1994</v>
           </cell>
+        </row>
+        <row r="25">
+          <cell r="C25"/>
+        </row>
+        <row r="26">
+          <cell r="C26"/>
+        </row>
+        <row r="27">
+          <cell r="C27"/>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="6">
+          <cell r="C6">
+            <v>33.75</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="C7">
+            <v>6.16</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="C8">
+            <v>207.9</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="C11">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="C12">
+            <v>207.9</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="C23" t="str">
+            <v>Paris, France</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="C24">
+            <v>1996</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="C27"/>
+        </row>
+        <row r="28">
+          <cell r="C28"/>
+        </row>
+        <row r="29">
+          <cell r="C29"/>
         </row>
       </sheetData>
     </sheetDataSet>
@@ -7785,13 +7879,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EA11F49-38A5-4A76-81B0-A144DE239010}">
-  <dimension ref="A1:AH21"/>
+  <dimension ref="A1:AJ21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
+      <selection pane="bottomRight" activeCell="T1" sqref="T1:T1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7801,20 +7895,24 @@
     <col min="3" max="3" width="30.28515625" style="43" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" style="43" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="43"/>
-    <col min="6" max="6" width="11.7109375" style="54" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="54" customWidth="1"/>
     <col min="7" max="10" width="9.140625" style="64"/>
-    <col min="11" max="12" width="9.140625" style="43"/>
+    <col min="11" max="12" width="9.140625" style="51"/>
     <col min="13" max="14" width="9.140625" style="61"/>
-    <col min="15" max="25" width="9.140625" style="43"/>
-    <col min="26" max="30" width="9.140625" style="54"/>
-    <col min="31" max="31" width="9.140625" style="43"/>
-    <col min="32" max="32" width="9.140625" style="51"/>
+    <col min="15" max="19" width="9.140625" style="43"/>
+    <col min="20" max="20" width="10.85546875" style="51" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.140625" style="43"/>
+    <col min="22" max="26" width="9.140625" style="51"/>
+    <col min="27" max="27" width="9.140625" style="43"/>
+    <col min="28" max="32" width="9.140625" style="54"/>
     <col min="33" max="33" width="9.140625" style="43"/>
-    <col min="34" max="34" width="14.7109375" style="43" bestFit="1" customWidth="1"/>
-    <col min="35" max="16384" width="9.140625" style="43"/>
+    <col min="34" max="34" width="9.140625" style="51"/>
+    <col min="35" max="35" width="9.140625" style="43"/>
+    <col min="36" max="36" width="14.7109375" style="43" bestFit="1" customWidth="1"/>
+    <col min="37" max="16384" width="9.140625" style="43"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
       <c r="F1" s="67" t="s">
         <v>616</v>
       </c>
@@ -7823,7 +7921,7 @@
       <c r="I1" s="67"/>
       <c r="J1" s="67"/>
     </row>
-    <row r="2" spans="1:34" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="43"/>
       <c r="B2" s="44" t="s">
         <v>567</v>
@@ -7875,63 +7973,66 @@
         <v>599</v>
       </c>
       <c r="T2" s="45" t="s">
+        <v>618</v>
+      </c>
+      <c r="V2" s="45" t="s">
         <v>604</v>
       </c>
-      <c r="U2" s="45" t="s">
+      <c r="W2" s="45" t="s">
         <v>605</v>
       </c>
-      <c r="V2" s="45" t="s">
+      <c r="X2" s="45" t="s">
         <v>609</v>
       </c>
-      <c r="W2" s="45" t="s">
+      <c r="Y2" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="X2" s="45" t="s">
+      <c r="Z2" s="45" t="s">
         <v>608</v>
       </c>
-      <c r="Z2" s="53" t="s">
+      <c r="AB2" s="53" t="s">
         <v>617</v>
       </c>
-      <c r="AA2" s="53" t="s">
+      <c r="AC2" s="53" t="s">
         <v>600</v>
       </c>
-      <c r="AB2" s="53" t="s">
+      <c r="AD2" s="53" t="s">
         <v>601</v>
       </c>
-      <c r="AC2" s="53" t="s">
+      <c r="AE2" s="53" t="s">
         <v>602</v>
       </c>
-      <c r="AD2" s="53" t="s">
+      <c r="AF2" s="53" t="s">
         <v>603</v>
       </c>
-      <c r="AF2" s="45" t="s">
+      <c r="AH2" s="45" t="s">
         <v>613</v>
       </c>
-      <c r="AG2" s="44" t="s">
+      <c r="AI2" s="44" t="s">
         <v>607</v>
       </c>
-      <c r="AH2" s="45" t="s">
+      <c r="AJ2" s="45" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="C3" s="46"/>
       <c r="D3" s="51"/>
       <c r="E3" s="51"/>
       <c r="P3" s="51"/>
       <c r="Q3" s="51"/>
       <c r="R3" s="51"/>
-      <c r="AG3" s="51"/>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI3" s="51"/>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="D4" s="51"/>
       <c r="E4" s="51"/>
       <c r="P4" s="51"/>
       <c r="Q4" s="51"/>
       <c r="R4" s="51"/>
-      <c r="AG4" s="51"/>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI4" s="51"/>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B5" s="43" t="s">
         <v>586</v>
       </c>
@@ -7947,9 +8048,9 @@
       <c r="P5" s="51"/>
       <c r="Q5" s="51"/>
       <c r="R5" s="51"/>
-      <c r="AG5" s="51"/>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI5" s="51"/>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B6" s="43" t="s">
         <v>577</v>
       </c>
@@ -7965,9 +8066,9 @@
       <c r="P6" s="51"/>
       <c r="Q6" s="51"/>
       <c r="R6" s="51"/>
-      <c r="AG6" s="51"/>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI6" s="51"/>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B7" s="52" t="s">
         <v>578</v>
       </c>
@@ -7981,38 +8082,38 @@
         <v>588</v>
       </c>
       <c r="F7" s="56">
-        <f>[4]Main!$C$6*E20</f>
+        <f>[1]Main!$C$6*E20</f>
         <v>113.46400000000001</v>
       </c>
       <c r="G7" s="64">
-        <f>[4]Main!$C$7</f>
+        <f>[1]Main!$C$7</f>
         <v>169.83</v>
       </c>
       <c r="H7" s="64">
-        <f>[4]Main!$C$8*E20</f>
+        <f>[1]Main!$C$8*E20</f>
         <v>19269.591120000005</v>
       </c>
       <c r="I7" s="64">
-        <f>[4]Main!$C$11*E20</f>
+        <f>[1]Main!$C$11*E20</f>
         <v>0</v>
       </c>
       <c r="J7" s="64">
-        <f>[4]Main!$C$12*E20</f>
+        <f>[1]Main!$C$12*E20</f>
         <v>19269.591120000005</v>
       </c>
       <c r="P7" s="51"/>
       <c r="Q7" s="51"/>
       <c r="R7" s="51"/>
-      <c r="AG7" s="51">
-        <f>[4]Main!$C$24</f>
+      <c r="AI7" s="51">
+        <f>[1]Main!$C$24</f>
         <v>1993</v>
       </c>
-      <c r="AH7" s="51" t="str">
-        <f>[4]Main!$C$23</f>
+      <c r="AJ7" s="51" t="str">
+        <f>[1]Main!$C$23</f>
         <v>NYC, NY</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B8" s="43" t="s">
         <v>81</v>
       </c>
@@ -8028,9 +8129,9 @@
       <c r="P8" s="51"/>
       <c r="Q8" s="51"/>
       <c r="R8" s="51"/>
-      <c r="AG8" s="51"/>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI8" s="51"/>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B9" s="43" t="s">
         <v>580</v>
       </c>
@@ -8046,9 +8147,9 @@
       <c r="P9" s="51"/>
       <c r="Q9" s="51"/>
       <c r="R9" s="51"/>
-      <c r="AG9" s="51"/>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI9" s="51"/>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B10" s="43" t="s">
         <v>127</v>
       </c>
@@ -8057,16 +8158,14 @@
       </c>
       <c r="D10" s="51"/>
       <c r="E10" s="51"/>
-      <c r="K10" s="51"/>
-      <c r="L10" s="51"/>
       <c r="M10" s="62"/>
       <c r="N10" s="62"/>
       <c r="O10" s="51"/>
       <c r="P10" s="51"/>
       <c r="Q10" s="51"/>
-      <c r="AG10" s="51"/>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI10" s="51"/>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B11" s="43" t="s">
         <v>186</v>
       </c>
@@ -8075,21 +8174,22 @@
       </c>
       <c r="D11" s="51"/>
       <c r="E11" s="51"/>
-      <c r="K11" s="51"/>
-      <c r="L11" s="51"/>
       <c r="M11" s="62"/>
       <c r="N11" s="62"/>
       <c r="O11" s="51"/>
       <c r="P11" s="51"/>
       <c r="Q11" s="51"/>
-      <c r="AG11" s="51"/>
-    </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI11" s="51"/>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A12" s="43" t="s">
+        <v>575</v>
+      </c>
       <c r="B12" s="52" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="C12" s="43" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="D12" s="51" t="s">
         <v>595</v>
@@ -8097,181 +8197,231 @@
       <c r="E12" s="51" t="s">
         <v>596</v>
       </c>
-      <c r="F12" s="55">
-        <f>[1]Main!$C$6</f>
-        <v>4.9249999999999998</v>
+      <c r="F12" s="54">
+        <f>[2]Main!$C$6</f>
+        <v>2.75</v>
+      </c>
+      <c r="G12" s="64">
+        <f>[2]Main!$C$7</f>
+        <v>145.80000000000001</v>
       </c>
       <c r="H12" s="64">
-        <f>[1]Main!$C$8</f>
-        <v>194.14349999999999</v>
+        <f>[2]Main!$C$8</f>
+        <v>400.95000000000005</v>
       </c>
       <c r="I12" s="64">
-        <f>[1]Main!$C$11</f>
+        <f>[2]Main!$C$11</f>
         <v>0</v>
       </c>
       <c r="J12" s="64">
-        <f>[1]Main!$C$12</f>
-        <v>194.14349999999999</v>
-      </c>
-      <c r="K12" s="51"/>
-      <c r="L12" s="51"/>
+        <f>[2]Main!$C$12</f>
+        <v>400.95000000000005</v>
+      </c>
+      <c r="K12" s="51" t="str">
+        <f>+[2]Main!$C$33</f>
+        <v>H123</v>
+      </c>
+      <c r="L12" s="68">
+        <f>+[2]Main!$D$33</f>
+        <v>45188</v>
+      </c>
       <c r="M12" s="62"/>
       <c r="N12" s="62"/>
       <c r="O12" s="51"/>
       <c r="P12" s="51">
-        <f>[1]Main!$C$25</f>
+        <f>[2]Main!$C$27</f>
         <v>0</v>
       </c>
       <c r="Q12" s="51">
-        <f>[1]Main!$C$26</f>
+        <f>[2]Main!$C$28</f>
         <v>0</v>
       </c>
       <c r="R12" s="51">
-        <f>[1]Main!$C$27</f>
+        <f>[2]Main!$C$29</f>
         <v>0</v>
       </c>
-      <c r="AG12" s="51">
-        <f>[1]Main!$C$24</f>
-        <v>1994</v>
-      </c>
-      <c r="AH12" s="51" t="str">
-        <f>[1]Main!$C$23</f>
-        <v>Cambridge, UK</v>
-      </c>
-    </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A13" s="43" t="s">
-        <v>575</v>
-      </c>
-      <c r="B13" s="43" t="s">
-        <v>202</v>
+      <c r="T12" s="51">
+        <f>+[2]Main!$C$31</f>
+        <v>438</v>
+      </c>
+      <c r="V12" s="69">
+        <f>+[2]Main!$C$38</f>
+        <v>1.5479168086347954</v>
+      </c>
+      <c r="AH12" s="51">
+        <f>[2]Main!$C$25</f>
+        <v>2018</v>
+      </c>
+      <c r="AI12" s="51">
+        <f>[2]Main!$C$24</f>
+        <v>1990</v>
+      </c>
+      <c r="AJ12" s="51" t="str">
+        <f>[2]Main!$C$23</f>
+        <v>Wakefield, UK</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B13" s="52" t="s">
+        <v>593</v>
       </c>
       <c r="C13" s="43" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="D13" s="51" t="s">
         <v>595</v>
       </c>
-      <c r="E13" s="51"/>
-      <c r="K13" s="51"/>
-      <c r="L13" s="51"/>
-      <c r="M13" s="62"/>
-      <c r="N13" s="62"/>
-      <c r="O13" s="51"/>
-      <c r="P13" s="51"/>
-      <c r="Q13" s="51"/>
-      <c r="AG13" s="51"/>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="E13" s="51" t="s">
+        <v>596</v>
+      </c>
+      <c r="F13" s="56">
+        <f>[3]Main!$C$6</f>
+        <v>1.155</v>
+      </c>
+      <c r="H13" s="64">
+        <f>[3]Main!$C$8</f>
+        <v>235.07715000000002</v>
+      </c>
+      <c r="I13" s="64">
+        <f>[3]Main!$C$11</f>
+        <v>0</v>
+      </c>
+      <c r="J13" s="64">
+        <f>[3]Main!$C$12</f>
+        <v>235.07715000000002</v>
+      </c>
+      <c r="P13" s="51">
+        <f>[3]Main!$C$25</f>
+        <v>10</v>
+      </c>
+      <c r="Q13" s="51">
+        <f>[3]Main!$C$26</f>
+        <v>70</v>
+      </c>
+      <c r="R13" s="51">
+        <f>[3]Main!$C$27</f>
+        <v>30</v>
+      </c>
+      <c r="AI13" s="51">
+        <f>[3]Main!$C$24</f>
+        <v>2011</v>
+      </c>
+      <c r="AJ13" s="51" t="str">
+        <f>[3]Main!$C$23</f>
+        <v>Washington, US</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B14" s="52" t="s">
-        <v>581</v>
+        <v>196</v>
       </c>
       <c r="C14" s="43" t="s">
-        <v>614</v>
+        <v>591</v>
       </c>
       <c r="D14" s="51" t="s">
-        <v>95</v>
+        <v>595</v>
       </c>
       <c r="E14" s="51" t="s">
-        <v>579</v>
-      </c>
-      <c r="F14" s="54">
-        <f>[2]Main!$C$6*E21</f>
-        <v>28.349999999999998</v>
-      </c>
-      <c r="G14" s="64">
-        <f>[2]Main!$C$7</f>
-        <v>6.16</v>
+        <v>596</v>
+      </c>
+      <c r="F14" s="55">
+        <f>[4]Main!$C$6</f>
+        <v>4.9249999999999998</v>
       </c>
       <c r="H14" s="64">
-        <f>[2]Main!$C$8*$E$21</f>
-        <v>174.636</v>
+        <f>[4]Main!$C$8</f>
+        <v>194.14349999999999</v>
       </c>
       <c r="I14" s="64">
-        <f>[2]Main!$C$11*$E$21</f>
+        <f>[4]Main!$C$11</f>
         <v>0</v>
       </c>
       <c r="J14" s="64">
-        <f>[2]Main!$C$12*$E$21</f>
-        <v>174.636</v>
-      </c>
-      <c r="K14" s="51"/>
-      <c r="L14" s="51"/>
+        <f>[4]Main!$C$12</f>
+        <v>194.14349999999999</v>
+      </c>
       <c r="M14" s="62"/>
       <c r="N14" s="62"/>
       <c r="O14" s="51"/>
       <c r="P14" s="51">
-        <f>[2]Main!$C$27</f>
+        <f>[4]Main!$C$25</f>
         <v>0</v>
       </c>
       <c r="Q14" s="51">
-        <f>[2]Main!$C$28</f>
+        <f>[4]Main!$C$26</f>
         <v>0</v>
       </c>
       <c r="R14" s="51">
-        <f>[2]Main!$C$29</f>
+        <f>[4]Main!$C$27</f>
         <v>0</v>
       </c>
-      <c r="AG14" s="51">
-        <f>[2]Main!$C$24</f>
+      <c r="AI14" s="51">
+        <f>[4]Main!$C$24</f>
+        <v>1994</v>
+      </c>
+      <c r="AJ14" s="51" t="str">
+        <f>[4]Main!$C$23</f>
+        <v>Cambridge, UK</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B15" s="52" t="s">
+        <v>581</v>
+      </c>
+      <c r="C15" s="43" t="s">
+        <v>614</v>
+      </c>
+      <c r="D15" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="E15" s="51" t="s">
+        <v>579</v>
+      </c>
+      <c r="F15" s="54">
+        <f>[5]Main!$C$6*E21</f>
+        <v>28.349999999999998</v>
+      </c>
+      <c r="G15" s="64">
+        <f>[5]Main!$C$7</f>
+        <v>6.16</v>
+      </c>
+      <c r="H15" s="64">
+        <f>[5]Main!$C$8*$E$21</f>
+        <v>174.636</v>
+      </c>
+      <c r="I15" s="64">
+        <f>[5]Main!$C$11*$E$21</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="64">
+        <f>[5]Main!$C$12*$E$21</f>
+        <v>174.636</v>
+      </c>
+      <c r="M15" s="62"/>
+      <c r="N15" s="62"/>
+      <c r="O15" s="51"/>
+      <c r="P15" s="51">
+        <f>[5]Main!$C$27</f>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="51">
+        <f>[5]Main!$C$28</f>
+        <v>0</v>
+      </c>
+      <c r="R15" s="51">
+        <f>[5]Main!$C$29</f>
+        <v>0</v>
+      </c>
+      <c r="AI15" s="51">
+        <f>[5]Main!$C$24</f>
         <v>1996</v>
       </c>
-      <c r="AH14" s="51" t="str">
-        <f>[2]Main!$C$23</f>
+      <c r="AJ15" s="51" t="str">
+        <f>[5]Main!$C$23</f>
         <v>Paris, France</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="B15" s="52" t="s">
-        <v>593</v>
-      </c>
-      <c r="C15" s="43" t="s">
-        <v>594</v>
-      </c>
-      <c r="D15" s="51" t="s">
-        <v>595</v>
-      </c>
-      <c r="E15" s="51" t="s">
-        <v>596</v>
-      </c>
-      <c r="F15" s="56">
-        <f>[3]Main!$C$6</f>
-        <v>1.155</v>
-      </c>
-      <c r="H15" s="64">
-        <f>[3]Main!$C$8</f>
-        <v>235.07715000000002</v>
-      </c>
-      <c r="I15" s="64">
-        <f>[3]Main!$C$11</f>
-        <v>0</v>
-      </c>
-      <c r="J15" s="64">
-        <f>[3]Main!$C$12</f>
-        <v>235.07715000000002</v>
-      </c>
-      <c r="P15" s="51">
-        <f>[3]Main!$C$25</f>
-        <v>10</v>
-      </c>
-      <c r="Q15" s="51">
-        <f>[3]Main!$C$26</f>
-        <v>70</v>
-      </c>
-      <c r="R15" s="51">
-        <f>[3]Main!$C$27</f>
-        <v>30</v>
-      </c>
-      <c r="AG15" s="51">
-        <f>[3]Main!$C$24</f>
-        <v>2011</v>
-      </c>
-      <c r="AH15" s="51" t="str">
-        <f>[3]Main!$C$23</f>
-        <v>Washington, US</v>
-      </c>
-    </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
       <c r="D16" s="51"/>
       <c r="E16" s="51"/>
     </row>
@@ -8314,12 +8464,13 @@
     <mergeCell ref="F1:J1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B15" r:id="rId1" xr:uid="{492A76F4-4882-4A78-B48A-FE2771E6353E}"/>
-    <hyperlink ref="B12" r:id="rId2" xr:uid="{FF627AC4-0649-433C-9977-CAE6BE5385C4}"/>
-    <hyperlink ref="B14" r:id="rId3" xr:uid="{7B76C08B-C15A-49CB-8685-38243193D2C8}"/>
+    <hyperlink ref="B13" r:id="rId1" xr:uid="{492A76F4-4882-4A78-B48A-FE2771E6353E}"/>
+    <hyperlink ref="B14" r:id="rId2" xr:uid="{FF627AC4-0649-433C-9977-CAE6BE5385C4}"/>
+    <hyperlink ref="B15" r:id="rId3" xr:uid="{7B76C08B-C15A-49CB-8685-38243193D2C8}"/>
     <hyperlink ref="B7" r:id="rId4" xr:uid="{D0C7F4E2-1E58-4B5D-A93E-35211C64E1BD}"/>
+    <hyperlink ref="B12" r:id="rId5" xr:uid="{2C0365FD-29AB-4B4C-B5D9-9DB5F0FDE789}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="125" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId5"/>
+  <pageSetup paperSize="125" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
£FDEV latest balance sheets
</commit_message>
<xml_diff>
--- a/Overview - Video Games.xlsx
+++ b/Overview - Video Games.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A3CCA2-5263-4170-BFF6-432839DABF60}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{807BBFE7-C7C4-44FC-833B-73660BDCE7F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{241F2393-9455-43D4-B289-8A800D465992}"/>
   </bookViews>
@@ -2584,6 +2584,12 @@
             <v>3</v>
           </cell>
         </row>
+        <row r="28">
+          <cell r="C28"/>
+        </row>
+        <row r="29">
+          <cell r="C29"/>
+        </row>
         <row r="31">
           <cell r="C31">
             <v>438</v>
@@ -2695,7 +2701,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2761,6 +2767,11 @@
           </cell>
           <cell r="D33">
             <v>45182</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="C38">
+            <v>0.84148858158761264</v>
           </cell>
         </row>
       </sheetData>
@@ -7944,10 +7955,10 @@
   <dimension ref="A1:AJ21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L23" sqref="L23"/>
+      <selection pane="bottomRight" activeCell="X19" sqref="X19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8475,6 +8486,26 @@
         <f>+[4]Main!$C$31</f>
         <v>915</v>
       </c>
+      <c r="V14" s="66">
+        <f>+[4]Main!$C$38</f>
+        <v>0.84148858158761264</v>
+      </c>
+      <c r="W14" s="66">
+        <f>+[4]Main!$C$39</f>
+        <v>0</v>
+      </c>
+      <c r="X14" s="66">
+        <f>+[4]Main!$C$40</f>
+        <v>0</v>
+      </c>
+      <c r="Y14" s="66">
+        <f>+[4]Main!$C$41</f>
+        <v>0</v>
+      </c>
+      <c r="Z14" s="66">
+        <f>+[4]Main!$C$42</f>
+        <v>0</v>
+      </c>
       <c r="AH14" s="51">
         <f>[4]Main!$C$25</f>
         <v>2013</v>

</xml_diff>